<commit_message>
Using Ben's results for file read time
they look more accurate.
</commit_message>
<xml_diff>
--- a/operations/4_file_system/file_read_time/logs/file_read_time_plots.xlsx
+++ b/operations/4_file_system/file_read_time/logs/file_read_time_plots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rohitgupta/Desktop/UCSD/quarter_4/cse_221/project/CSE221_project/operations/4_file_system/file_read_time/logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14394A8-CF6E-114B-8ED7-CBBFF7666867}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76BA35D0-073B-4D4B-8D57-3112AEFB8D7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{0346AA52-3F2D-F046-8D9C-B2F2F9D318FC}"/>
   </bookViews>
@@ -58,19 +58,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF2FFF12"/>
-      <name val="Andale Mono"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -93,9 +87,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -272,64 +265,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>20.149422147122063</c:v>
+                  <c:v>20.232833109702931</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.842292022505948</c:v>
+                  <c:v>19.744975047186863</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.809020717565442</c:v>
+                  <c:v>18.977017131915751</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.043059333631927</c:v>
+                  <c:v>18.49465248812416</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.558061908282554</c:v>
+                  <c:v>18.668639187866518</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17.068211465564371</c:v>
+                  <c:v>18.358977363632651</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15.9054105106765</c:v>
+                  <c:v>18.566369979720218</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15.319213444864149</c:v>
+                  <c:v>18.348918297536347</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17.006074005687804</c:v>
+                  <c:v>15.526652058906944</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16.787162866188417</c:v>
+                  <c:v>15.574150007825725</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15.863290954887042</c:v>
+                  <c:v>15.344157180569118</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>15.385087202081992</c:v>
+                  <c:v>15.35545433903599</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>16.415296138000667</c:v>
+                  <c:v>14.913730912257195</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>16.150342298919149</c:v>
+                  <c:v>15.696288387192</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>15.959503928032264</c:v>
+                  <c:v>15.149747119504683</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>16.237788805188259</c:v>
+                  <c:v>15.049508251055096</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>15.518898992777315</c:v>
+                  <c:v>15.129564765806499</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>15.666834244701487</c:v>
+                  <c:v>15.304280012316866</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>17.287477922555158</c:v>
+                  <c:v>15.323160340131725</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>15.235415935602527</c:v>
+                  <c:v>14.906373913076836</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -724,64 +717,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>20.149422147122063</c:v>
+                  <c:v>20.232833109702931</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.842292022505948</c:v>
+                  <c:v>19.744975047186863</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.809020717565442</c:v>
+                  <c:v>18.977017131915751</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.043059333631927</c:v>
+                  <c:v>18.49465248812416</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.558061908282554</c:v>
+                  <c:v>18.668639187866518</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17.068211465564371</c:v>
+                  <c:v>18.358977363632651</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15.9054105106765</c:v>
+                  <c:v>18.566369979720218</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15.319213444864149</c:v>
+                  <c:v>18.348918297536347</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17.006074005687804</c:v>
+                  <c:v>15.526652058906944</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16.787162866188417</c:v>
+                  <c:v>15.574150007825725</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15.863290954887042</c:v>
+                  <c:v>15.344157180569118</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>15.385087202081992</c:v>
+                  <c:v>15.35545433903599</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>16.415296138000667</c:v>
+                  <c:v>14.913730912257195</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>16.150342298919149</c:v>
+                  <c:v>15.696288387192</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>15.959503928032264</c:v>
+                  <c:v>15.149747119504683</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>16.237788805188259</c:v>
+                  <c:v>15.049508251055096</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>15.518898992777315</c:v>
+                  <c:v>15.129564765806499</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>15.666834244701487</c:v>
+                  <c:v>15.304280012316866</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>17.287477922555158</c:v>
+                  <c:v>15.323160340131725</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>15.235415935602527</c:v>
+                  <c:v>14.906373913076836</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -907,64 +900,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>19.789885424558516</c:v>
+                  <c:v>19.920488066843955</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.826489524069181</c:v>
+                  <c:v>18.904131834429794</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.744919221753168</c:v>
+                  <c:v>18.951825396580418</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.98267055375678</c:v>
+                  <c:v>18.383003899761178</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.955218523714688</c:v>
+                  <c:v>18.27364992394369</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15.705497398351643</c:v>
+                  <c:v>17.657974324726641</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15.547527187843452</c:v>
+                  <c:v>17.706327380811651</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16.200017335880428</c:v>
+                  <c:v>17.60304673988383</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>16.43836953222641</c:v>
+                  <c:v>15.583464786581265</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>15.842252117368433</c:v>
+                  <c:v>15.672646326124626</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15.70439001178843</c:v>
+                  <c:v>15.626479063971249</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>16.498662252248717</c:v>
+                  <c:v>15.4594636383246</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>15.907594864619764</c:v>
+                  <c:v>15.239971386109257</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>16.043817643431499</c:v>
+                  <c:v>15.352871054677996</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>16.25146391820472</c:v>
+                  <c:v>15.202085551489173</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>16.529278028424621</c:v>
+                  <c:v>15.416863486917576</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>15.691689002760329</c:v>
+                  <c:v>15.23511671439625</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>15.858053866487632</c:v>
+                  <c:v>15.430909855325313</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>15.587631036442524</c:v>
+                  <c:v>15.640018932455787</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>15.379446059507211</c:v>
+                  <c:v>15.082149041353873</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -991,6 +984,790 @@
         <c:axId val="324618032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="16"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>log</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> base2 of file sizes (bytes)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="378345888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="378345888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="14"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>log base2 of access times (clock cycles)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="324618032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Local File Read</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> Time</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>random</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>29.000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>31.000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>31.584962500721158</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>32.321928094887362</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>32.584962500721154</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>32.807354922057606</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$3:$D$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>20.232833109702931</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19.744975047186863</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18.977017131915751</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18.49465248812416</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.668639187866518</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18.358977363632651</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18.566369979720218</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18.348918297536347</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.526652058906944</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15.574150007825725</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15.344157180569118</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15.35545433903599</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14.913730912257195</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15.696288387192</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.149747119504683</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15.049508251055096</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15.129564765806499</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>15.304280012316866</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>15.323160340131725</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>14.906373913076836</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-28A6-6042-9D13-05BD4AC501CF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>sequential</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>29.000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>31.000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>31.584962500721158</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>32.321928094887362</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>32.584962500721154</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>32.807354922057606</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$M$3:$M$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>19.920488066843955</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18.904131834429794</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18.951825396580418</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18.383003899761178</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.27364992394369</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17.657974324726641</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17.706327380811651</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17.60304673988383</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.583464786581265</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15.672646326124626</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15.626479063971249</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15.4594636383246</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>15.239971386109257</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15.352871054677996</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.202085551489173</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15.416863486917576</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15.23511671439625</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>15.430909855325313</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>15.640018932455787</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>15.082149041353873</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-28A6-6042-9D13-05BD4AC501CF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="324618032"/>
+        <c:axId val="378345888"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="324618032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="24"/>
           <c:min val="16"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1393,6 +2170,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1910,6 +2727,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2494,6 +3827,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6AD79942-29CB-8C4B-B0B3-0B13A0F34939}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2801,8 +4172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2590BD56-2612-DD42-8A10-B8A6AACC1227}">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="F21" workbookViewId="0">
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2814,42 +4185,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="J1" s="3" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="J1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2861,12 +4232,12 @@
         <f>LOG(1024*A3, 2)</f>
         <v>17</v>
       </c>
-      <c r="C3" s="1">
-        <v>1163002</v>
+      <c r="C3">
+        <v>1232224</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D5" si="0">LOG(C3,2)</f>
-        <v>20.149422147122063</v>
+        <v>20.232833109702931</v>
       </c>
       <c r="J3">
         <v>128</v>
@@ -2875,12 +4246,12 @@
         <f>LOG(1024*J3, 2)</f>
         <v>17</v>
       </c>
-      <c r="L3" s="1">
-        <v>906461</v>
+      <c r="L3">
+        <v>992349</v>
       </c>
       <c r="M3">
         <f t="shared" ref="M3:M5" si="1">LOG(L3,2)</f>
-        <v>19.789885424558516</v>
+        <v>19.920488066843955</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -2891,12 +4262,12 @@
         <f t="shared" ref="B4:B5" si="2">LOG(1024*A4, 2)</f>
         <v>18</v>
       </c>
-      <c r="C4" s="1">
-        <v>469997</v>
+      <c r="C4">
+        <v>878678</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>18.842292022505948</v>
+        <v>19.744975047186863</v>
       </c>
       <c r="J4">
         <v>256</v>
@@ -2905,12 +4276,12 @@
         <f t="shared" ref="K4:K5" si="3">LOG(1024*J4, 2)</f>
         <v>18</v>
       </c>
-      <c r="L4" s="1">
-        <v>464877</v>
+      <c r="L4">
+        <v>490581</v>
       </c>
       <c r="M4">
         <f t="shared" si="1"/>
-        <v>18.826489524069181</v>
+        <v>18.904131834429794</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -2921,12 +4292,12 @@
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="C5" s="1">
-        <v>229641</v>
+      <c r="C5">
+        <v>516002</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>17.809020717565442</v>
+        <v>18.977017131915751</v>
       </c>
       <c r="J5">
         <v>512</v>
@@ -2935,12 +4306,12 @@
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="L5" s="1">
-        <v>219661</v>
+      <c r="L5">
+        <v>507070</v>
       </c>
       <c r="M5">
         <f t="shared" si="1"/>
-        <v>17.744919221753168</v>
+        <v>18.951825396580418</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -2951,12 +4322,12 @@
         <f>LOG(A6*1024*1024,2)</f>
         <v>20</v>
       </c>
-      <c r="C6" s="1">
-        <v>135043</v>
+      <c r="C6">
+        <v>369356</v>
       </c>
       <c r="D6">
         <f>LOG(C6,2)</f>
-        <v>17.043059333631927</v>
+        <v>18.49465248812416</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -2965,12 +4336,12 @@
         <f>LOG(J6*1024*1024,2)</f>
         <v>20</v>
       </c>
-      <c r="L6" s="1">
-        <v>259014</v>
+      <c r="L6">
+        <v>341850</v>
       </c>
       <c r="M6">
         <f>LOG(L6,2)</f>
-        <v>17.98267055375678</v>
+        <v>18.383003899761178</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -2981,12 +4352,12 @@
         <f t="shared" ref="B7:B22" si="4">LOG(A7*1024*1024,2)</f>
         <v>21</v>
       </c>
-      <c r="C7" s="1">
-        <v>96488</v>
+      <c r="C7">
+        <v>416697</v>
       </c>
       <c r="D7">
         <f t="shared" ref="D7:D22" si="5">LOG(C7,2)</f>
-        <v>16.558061908282554</v>
+        <v>18.668639187866518</v>
       </c>
       <c r="J7">
         <v>2</v>
@@ -2995,12 +4366,12 @@
         <f t="shared" ref="K7:K22" si="6">LOG(J7*1024*1024,2)</f>
         <v>21</v>
       </c>
-      <c r="L7" s="1">
-        <v>127066</v>
+      <c r="L7">
+        <v>316896</v>
       </c>
       <c r="M7">
         <f t="shared" ref="M7:M22" si="7">LOG(L7,2)</f>
-        <v>16.955218523714688</v>
+        <v>18.27364992394369</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -3011,12 +4382,12 @@
         <f t="shared" si="4"/>
         <v>22</v>
       </c>
-      <c r="C8" s="1">
-        <v>137418</v>
+      <c r="C8">
+        <v>336204</v>
       </c>
       <c r="D8">
         <f t="shared" si="5"/>
-        <v>17.068211465564371</v>
+        <v>18.358977363632651</v>
       </c>
       <c r="J8">
         <v>4</v>
@@ -3025,12 +4396,12 @@
         <f t="shared" si="6"/>
         <v>22</v>
       </c>
-      <c r="L8" s="1">
-        <v>53435</v>
+      <c r="L8">
+        <v>206814</v>
       </c>
       <c r="M8">
         <f t="shared" si="7"/>
-        <v>15.705497398351643</v>
+        <v>17.657974324726641</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -3041,12 +4412,12 @@
         <f t="shared" si="4"/>
         <v>23</v>
       </c>
-      <c r="C9" s="1">
-        <v>61377</v>
+      <c r="C9">
+        <v>388181</v>
       </c>
       <c r="D9">
         <f t="shared" si="5"/>
-        <v>15.9054105106765</v>
+        <v>18.566369979720218</v>
       </c>
       <c r="J9">
         <v>8</v>
@@ -3055,12 +4426,12 @@
         <f t="shared" si="6"/>
         <v>23</v>
       </c>
-      <c r="L9" s="1">
-        <v>47893</v>
+      <c r="L9">
+        <v>213863</v>
       </c>
       <c r="M9">
         <f t="shared" si="7"/>
-        <v>15.547527187843452</v>
+        <v>17.706327380811651</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -3071,12 +4442,12 @@
         <f t="shared" si="4"/>
         <v>24</v>
       </c>
-      <c r="C10" s="1">
-        <v>40883</v>
+      <c r="C10">
+        <v>333868</v>
       </c>
       <c r="D10">
         <f t="shared" si="5"/>
-        <v>15.319213444864149</v>
+        <v>18.348918297536347</v>
       </c>
       <c r="J10">
         <v>16</v>
@@ -3085,12 +4456,12 @@
         <f t="shared" si="6"/>
         <v>24</v>
       </c>
-      <c r="L10" s="1">
-        <v>75282</v>
+      <c r="L10">
+        <v>199088</v>
       </c>
       <c r="M10">
         <f t="shared" si="7"/>
-        <v>16.200017335880428</v>
+        <v>17.60304673988383</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -3101,12 +4472,12 @@
         <f t="shared" si="4"/>
         <v>25</v>
       </c>
-      <c r="C11" s="1">
-        <v>131625</v>
+      <c r="C11">
+        <v>47205</v>
       </c>
       <c r="D11">
         <f t="shared" si="5"/>
-        <v>17.006074005687804</v>
+        <v>15.526652058906944</v>
       </c>
       <c r="J11">
         <v>32</v>
@@ -3115,12 +4486,12 @@
         <f t="shared" si="6"/>
         <v>25</v>
       </c>
-      <c r="L11" s="1">
-        <v>88806</v>
+      <c r="L11">
+        <v>49101</v>
       </c>
       <c r="M11">
         <f t="shared" si="7"/>
-        <v>16.43836953222641</v>
+        <v>15.583464786581265</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -3131,12 +4502,12 @@
         <f t="shared" si="4"/>
         <v>26</v>
       </c>
-      <c r="C12" s="1">
-        <v>113094</v>
+      <c r="C12">
+        <v>48785</v>
       </c>
       <c r="D12">
         <f t="shared" si="5"/>
-        <v>16.787162866188417</v>
+        <v>15.574150007825725</v>
       </c>
       <c r="J12">
         <v>64</v>
@@ -3145,12 +4516,12 @@
         <f t="shared" si="6"/>
         <v>26</v>
       </c>
-      <c r="L12" s="1">
-        <v>58748</v>
+      <c r="L12">
+        <v>52232</v>
       </c>
       <c r="M12">
         <f t="shared" si="7"/>
-        <v>15.842252117368433</v>
+        <v>15.672646326124626</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -3161,12 +4532,12 @@
         <f t="shared" si="4"/>
         <v>27</v>
       </c>
-      <c r="C13" s="1">
-        <v>59611</v>
+      <c r="C13">
+        <v>41596</v>
       </c>
       <c r="D13">
         <f t="shared" si="5"/>
-        <v>15.863290954887042</v>
+        <v>15.344157180569118</v>
       </c>
       <c r="J13">
         <v>128</v>
@@ -3175,12 +4546,12 @@
         <f t="shared" si="6"/>
         <v>27</v>
       </c>
-      <c r="L13" s="1">
-        <v>53394</v>
+      <c r="L13">
+        <v>50587</v>
       </c>
       <c r="M13">
         <f t="shared" si="7"/>
-        <v>15.70439001178843</v>
+        <v>15.626479063971249</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -3191,12 +4562,12 @@
         <f t="shared" si="4"/>
         <v>28</v>
       </c>
-      <c r="C14" s="1">
-        <v>42793</v>
+      <c r="C14">
+        <v>41923</v>
       </c>
       <c r="D14">
         <f t="shared" si="5"/>
-        <v>15.385087202081992</v>
+        <v>15.35545433903599</v>
       </c>
       <c r="J14">
         <v>256</v>
@@ -3205,12 +4576,12 @@
         <f t="shared" si="6"/>
         <v>28</v>
       </c>
-      <c r="L14" s="1">
-        <v>92596</v>
+      <c r="L14">
+        <v>45057</v>
       </c>
       <c r="M14">
         <f t="shared" si="7"/>
-        <v>16.498662252248717</v>
+        <v>15.4594636383246</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -3221,12 +4592,12 @@
         <f t="shared" si="4"/>
         <v>29.000000000000004</v>
       </c>
-      <c r="C15" s="1">
-        <v>87397</v>
+      <c r="C15">
+        <v>30866</v>
       </c>
       <c r="D15">
         <f t="shared" si="5"/>
-        <v>16.415296138000667</v>
+        <v>14.913730912257195</v>
       </c>
       <c r="J15">
         <v>512</v>
@@ -3235,12 +4606,12 @@
         <f t="shared" si="6"/>
         <v>29.000000000000004</v>
       </c>
-      <c r="L15" s="1">
-        <v>61470</v>
+      <c r="L15">
+        <v>38698</v>
       </c>
       <c r="M15">
         <f t="shared" si="7"/>
-        <v>15.907594864619764</v>
+        <v>15.239971386109257</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -3251,12 +4622,12 @@
         <f t="shared" si="4"/>
         <v>30</v>
       </c>
-      <c r="C16" s="1">
-        <v>72734</v>
+      <c r="C16">
+        <v>53095</v>
       </c>
       <c r="D16">
         <f t="shared" si="5"/>
-        <v>16.150342298919149</v>
+        <v>15.696288387192</v>
       </c>
       <c r="J16">
         <v>1024</v>
@@ -3265,12 +4636,12 @@
         <f t="shared" si="6"/>
         <v>30</v>
       </c>
-      <c r="L16" s="1">
-        <v>67557</v>
+      <c r="L16">
+        <v>41848</v>
       </c>
       <c r="M16">
         <f t="shared" si="7"/>
-        <v>16.043817643431499</v>
+        <v>15.352871054677996</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
@@ -3281,12 +4652,12 @@
         <f t="shared" si="4"/>
         <v>31.000000000000004</v>
       </c>
-      <c r="C17" s="1">
-        <v>63722</v>
+      <c r="C17">
+        <v>36352</v>
       </c>
       <c r="D17">
         <f t="shared" si="5"/>
-        <v>15.959503928032264</v>
+        <v>15.149747119504683</v>
       </c>
       <c r="J17">
         <v>2048</v>
@@ -3295,12 +4666,12 @@
         <f t="shared" si="6"/>
         <v>31.000000000000004</v>
       </c>
-      <c r="L17" s="1">
-        <v>78015</v>
+      <c r="L17">
+        <v>37695</v>
       </c>
       <c r="M17">
         <f t="shared" si="7"/>
-        <v>16.25146391820472</v>
+        <v>15.202085551489173</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
@@ -3311,12 +4682,12 @@
         <f t="shared" si="4"/>
         <v>31.584962500721158</v>
       </c>
-      <c r="C18" s="1">
-        <v>77279</v>
+      <c r="C18">
+        <v>33912</v>
       </c>
       <c r="D18">
         <f t="shared" si="5"/>
-        <v>16.237788805188259</v>
+        <v>15.049508251055096</v>
       </c>
       <c r="J18">
         <v>3072</v>
@@ -3325,12 +4696,12 @@
         <f t="shared" si="6"/>
         <v>31.584962500721158</v>
       </c>
-      <c r="L18" s="1">
-        <v>94582</v>
+      <c r="L18">
+        <v>43746</v>
       </c>
       <c r="M18">
         <f t="shared" si="7"/>
-        <v>16.529278028424621</v>
+        <v>15.416863486917576</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
@@ -3341,12 +4712,12 @@
         <f t="shared" si="4"/>
         <v>32</v>
       </c>
-      <c r="C19" s="1">
-        <v>46952</v>
+      <c r="C19">
+        <v>35847</v>
       </c>
       <c r="D19">
         <f t="shared" si="5"/>
-        <v>15.518898992777315</v>
+        <v>15.129564765806499</v>
       </c>
       <c r="J19">
         <v>4096</v>
@@ -3355,12 +4726,12 @@
         <f t="shared" si="6"/>
         <v>32</v>
       </c>
-      <c r="L19" s="1">
-        <v>52926</v>
+      <c r="L19">
+        <v>38568</v>
       </c>
       <c r="M19">
         <f t="shared" si="7"/>
-        <v>15.691689002760329</v>
+        <v>15.23511671439625</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
@@ -3371,12 +4742,12 @@
         <f t="shared" si="4"/>
         <v>32.321928094887362</v>
       </c>
-      <c r="C20" s="1">
-        <v>52022</v>
+      <c r="C20">
+        <v>40462</v>
       </c>
       <c r="D20">
         <f t="shared" si="5"/>
-        <v>15.666834244701487</v>
+        <v>15.304280012316866</v>
       </c>
       <c r="J20">
         <v>5120</v>
@@ -3385,12 +4756,12 @@
         <f t="shared" si="6"/>
         <v>32.321928094887362</v>
       </c>
-      <c r="L20" s="1">
-        <v>59395</v>
+      <c r="L20">
+        <v>44174</v>
       </c>
       <c r="M20">
         <f t="shared" si="7"/>
-        <v>15.858053866487632</v>
+        <v>15.430909855325313</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
@@ -3401,12 +4772,12 @@
         <f t="shared" si="4"/>
         <v>32.584962500721154</v>
       </c>
-      <c r="C21" s="1">
-        <v>159974</v>
+      <c r="C21">
+        <v>40995</v>
       </c>
       <c r="D21">
         <f t="shared" si="5"/>
-        <v>17.287477922555158</v>
+        <v>15.323160340131725</v>
       </c>
       <c r="J21">
         <v>6144</v>
@@ -3415,12 +4786,12 @@
         <f t="shared" si="6"/>
         <v>32.584962500721154</v>
       </c>
-      <c r="L21" s="1">
-        <v>49243</v>
+      <c r="L21">
+        <v>51064</v>
       </c>
       <c r="M21">
         <f t="shared" si="7"/>
-        <v>15.587631036442524</v>
+        <v>15.640018932455787</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
@@ -3431,12 +4802,12 @@
         <f t="shared" si="4"/>
         <v>32.807354922057606</v>
       </c>
-      <c r="C22" s="1">
-        <v>38576</v>
+      <c r="C22">
+        <v>30709</v>
       </c>
       <c r="D22">
         <f t="shared" si="5"/>
-        <v>15.235415935602527</v>
+        <v>14.906373913076836</v>
       </c>
       <c r="J22">
         <v>7168</v>
@@ -3445,12 +4816,12 @@
         <f t="shared" si="6"/>
         <v>32.807354922057606</v>
       </c>
-      <c r="L22" s="1">
-        <v>42626</v>
+      <c r="L22">
+        <v>34688</v>
       </c>
       <c r="M22">
         <f t="shared" si="7"/>
-        <v>15.379446059507211</v>
+        <v>15.082149041353873</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding script to run all (no remote) experiments
</commit_message>
<xml_diff>
--- a/operations/4_file_system/file_read_time/logs/file_read_time_plots.xlsx
+++ b/operations/4_file_system/file_read_time/logs/file_read_time_plots.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rohitgupta/Desktop/UCSD/quarter_4/cse_221/project/CSE221_project/operations/4_file_system/file_read_time/logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76BA35D0-073B-4D4B-8D57-3112AEFB8D7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B774D85-1701-E74C-B54B-19974DD85A7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{0346AA52-3F2D-F046-8D9C-B2F2F9D318FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -4172,7 +4172,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2590BD56-2612-DD42-8A10-B8A6AACC1227}">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F21" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G16" workbookViewId="0">
       <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>

</xml_diff>